<commit_message>
Aggiunto salvataggio Mar su verbale
</commit_message>
<xml_diff>
--- a/other/T0XXX.xlsx
+++ b/other/T0XXX.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\progetti\Interfaccia Mu.De. Manager\Mu.De.Manager\sv_Mu.De.Manager\Mu.De._Manager\other\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Progetti\Interfaccia Mu.De. Manager\Mu.De.Manager\sv_Mu.De.Manager\Mu.De._Manager\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBEBDBE-71E4-4664-AD20-64E898F0A26B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49509EFC-F874-4516-9BB4-18CD83EFC4C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="480" windowWidth="17115" windowHeight="8790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="46">
   <si>
     <t>F.P.</t>
   </si>
@@ -539,7 +539,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -764,77 +764,83 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1668,7 +1674,7 @@
   <dimension ref="A1:O54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1689,26 +1695,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="100"/>
-      <c r="B1" s="100"/>
-      <c r="C1" s="101" t="s">
+      <c r="A1" s="99"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="100" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="101"/>
-      <c r="E1" s="101"/>
-      <c r="F1" s="101"/>
-      <c r="G1" s="101"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
     </row>
     <row r="2" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="27"/>
       <c r="B2" s="27"/>
       <c r="C2" s="28"/>
       <c r="D2" s="28"/>
-      <c r="E2" s="105" t="s">
+      <c r="E2" s="104" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="105"/>
-      <c r="G2" s="105"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="104"/>
     </row>
     <row r="3" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="70" t="s">
@@ -1718,24 +1724,24 @@
         <v>12</v>
       </c>
       <c r="C3" s="30"/>
-      <c r="D3" s="98" t="s">
+      <c r="D3" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
       <c r="G3" s="49" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="31"/>
-      <c r="B4" s="106" t="s">
+      <c r="B4" s="105" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="106"/>
-      <c r="D4" s="106"/>
-      <c r="E4" s="106"/>
-      <c r="F4" s="106"/>
+      <c r="C4" s="105"/>
+      <c r="D4" s="105"/>
+      <c r="E4" s="105"/>
+      <c r="F4" s="105"/>
       <c r="G4" s="50"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -1751,15 +1757,15 @@
       <c r="G5" s="38"/>
     </row>
     <row r="6" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="102" t="s">
+      <c r="A6" s="101" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="103"/>
-      <c r="C6" s="103"/>
-      <c r="D6" s="103"/>
-      <c r="E6" s="103"/>
-      <c r="F6" s="103"/>
-      <c r="G6" s="104"/>
+      <c r="B6" s="102"/>
+      <c r="C6" s="102"/>
+      <c r="D6" s="102"/>
+      <c r="E6" s="102"/>
+      <c r="F6" s="102"/>
+      <c r="G6" s="103"/>
     </row>
     <row r="7" spans="1:10" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
@@ -1785,9 +1791,9 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="99"/>
-      <c r="B9" s="99"/>
-      <c r="C9" s="99"/>
+      <c r="A9" s="98"/>
+      <c r="B9" s="98"/>
+      <c r="C9" s="98"/>
       <c r="D9" s="10"/>
       <c r="E9" s="51"/>
       <c r="F9" s="6"/>
@@ -1809,9 +1815,9 @@
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="99"/>
-      <c r="B11" s="99"/>
-      <c r="C11" s="99"/>
+      <c r="A11" s="98"/>
+      <c r="B11" s="98"/>
+      <c r="C11" s="98"/>
       <c r="D11" s="10"/>
       <c r="E11" s="51"/>
       <c r="F11" s="6"/>
@@ -1833,9 +1839,9 @@
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="99"/>
-      <c r="B13" s="99"/>
-      <c r="C13" s="99"/>
+      <c r="A13" s="98"/>
+      <c r="B13" s="98"/>
+      <c r="C13" s="98"/>
       <c r="D13" s="10"/>
       <c r="E13" s="51"/>
       <c r="F13" s="6"/>
@@ -1843,10 +1849,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="25"/>
-      <c r="B14" s="97" t="s">
+      <c r="B14" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="97"/>
+      <c r="C14" s="96"/>
       <c r="D14" s="12" t="s">
         <v>6</v>
       </c>
@@ -1871,10 +1877,10 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="25"/>
-      <c r="B16" s="97" t="s">
+      <c r="B16" s="96" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="97"/>
+      <c r="C16" s="96"/>
       <c r="D16" s="12" t="s">
         <v>6</v>
       </c>
@@ -1889,9 +1895,9 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="99"/>
-      <c r="B17" s="99"/>
-      <c r="C17" s="99"/>
+      <c r="A17" s="98"/>
+      <c r="B17" s="98"/>
+      <c r="C17" s="98"/>
       <c r="D17" s="10"/>
       <c r="E17" s="51"/>
       <c r="F17" s="6"/>
@@ -1901,10 +1907,10 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="25"/>
-      <c r="B18" s="97" t="s">
+      <c r="B18" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="97"/>
+      <c r="C18" s="96"/>
       <c r="D18" s="21" t="s">
         <v>10</v>
       </c>
@@ -1932,15 +1938,15 @@
       <c r="L19" s="57"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="108"/>
-      <c r="B20" s="108"/>
-      <c r="C20" s="108"/>
+      <c r="A20" s="107"/>
+      <c r="B20" s="107"/>
+      <c r="C20" s="107"/>
       <c r="D20" s="7"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="107"/>
-      <c r="I20" s="107"/>
+      <c r="H20" s="106"/>
+      <c r="I20" s="106"/>
       <c r="J20" s="57"/>
       <c r="L20" s="57"/>
     </row>
@@ -1957,10 +1963,10 @@
       <c r="D21" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="118" t="s">
+      <c r="E21" s="117" t="s">
         <v>38</v>
       </c>
-      <c r="F21" s="119"/>
+      <c r="F21" s="118"/>
       <c r="G21" s="88" t="s">
         <v>39</v>
       </c>
@@ -2227,7 +2233,7 @@
       <c r="I29" s="87">
         <v>4100</v>
       </c>
-      <c r="J29" s="96"/>
+      <c r="J29" s="119"/>
       <c r="L29" s="57"/>
       <c r="M29"/>
     </row>
@@ -2241,7 +2247,9 @@
       <c r="G30" s="80"/>
       <c r="H30" s="82"/>
       <c r="I30" s="93"/>
-      <c r="J30" s="57"/>
+      <c r="J30" s="120" t="s">
+        <v>26</v>
+      </c>
       <c r="L30" s="57"/>
       <c r="M30"/>
     </row>
@@ -2302,7 +2310,7 @@
       <c r="H32" s="82">
         <v>3200</v>
       </c>
-      <c r="I32" s="86">
+      <c r="I32" s="82">
         <v>3700</v>
       </c>
       <c r="J32" s="95"/>
@@ -2337,7 +2345,7 @@
       <c r="I33" s="86">
         <v>3900</v>
       </c>
-      <c r="J33" s="95"/>
+      <c r="J33" s="121"/>
       <c r="L33" s="57"/>
       <c r="M33"/>
     </row>
@@ -2369,7 +2377,7 @@
       <c r="I34" s="86">
         <v>3900</v>
       </c>
-      <c r="J34" s="95"/>
+      <c r="J34" s="121"/>
       <c r="L34" s="57"/>
       <c r="M34"/>
     </row>
@@ -2401,7 +2409,7 @@
       <c r="I35" s="86">
         <v>4000</v>
       </c>
-      <c r="J35" s="95"/>
+      <c r="J35" s="121"/>
       <c r="L35" s="57"/>
       <c r="M35"/>
     </row>
@@ -2433,7 +2441,7 @@
       <c r="I36" s="86">
         <v>4000</v>
       </c>
-      <c r="J36" s="95"/>
+      <c r="J36" s="121"/>
       <c r="L36" s="57"/>
       <c r="M36"/>
     </row>
@@ -2465,7 +2473,7 @@
       <c r="I37" s="86">
         <v>4200</v>
       </c>
-      <c r="J37" s="95"/>
+      <c r="J37" s="121"/>
       <c r="L37" s="57"/>
       <c r="M37"/>
     </row>
@@ -2497,7 +2505,7 @@
       <c r="I38" s="86">
         <v>4300</v>
       </c>
-      <c r="J38" s="95"/>
+      <c r="J38" s="121"/>
       <c r="L38" s="57"/>
       <c r="M38"/>
     </row>
@@ -2526,7 +2534,7 @@
       <c r="H39" s="82">
         <v>3400</v>
       </c>
-      <c r="I39" s="86">
+      <c r="I39" s="82">
         <v>4200</v>
       </c>
       <c r="J39" s="95"/>
@@ -2561,7 +2569,7 @@
       <c r="I40" s="87">
         <v>4300</v>
       </c>
-      <c r="J40" s="96"/>
+      <c r="J40" s="119"/>
       <c r="L40" s="57"/>
       <c r="M40"/>
     </row>
@@ -2578,27 +2586,27 @@
     </row>
     <row r="42" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="43"/>
-      <c r="B42" s="117" t="s">
+      <c r="B42" s="116" t="s">
         <v>16</v>
       </c>
-      <c r="C42" s="117"/>
-      <c r="D42" s="117"/>
-      <c r="E42" s="117"/>
-      <c r="F42" s="117"/>
-      <c r="G42" s="117"/>
+      <c r="C42" s="116"/>
+      <c r="D42" s="116"/>
+      <c r="E42" s="116"/>
+      <c r="F42" s="116"/>
+      <c r="G42" s="116"/>
       <c r="H42" s="40"/>
       <c r="I42" s="41"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A43" s="112" t="s">
+      <c r="A43" s="111" t="s">
         <v>34</v>
       </c>
-      <c r="B43" s="113"/>
-      <c r="C43" s="113"/>
-      <c r="D43" s="111" t="s">
+      <c r="B43" s="112"/>
+      <c r="C43" s="112"/>
+      <c r="D43" s="110" t="s">
         <v>17</v>
       </c>
-      <c r="E43" s="111"/>
+      <c r="E43" s="110"/>
       <c r="F43" s="7" t="s">
         <v>19</v>
       </c>
@@ -2608,15 +2616,15 @@
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A44" s="114" t="s">
+      <c r="A44" s="113" t="s">
         <v>18</v>
       </c>
-      <c r="B44" s="115"/>
-      <c r="C44" s="115"/>
-      <c r="D44" s="116" t="s">
+      <c r="B44" s="114"/>
+      <c r="C44" s="114"/>
+      <c r="D44" s="115" t="s">
         <v>20</v>
       </c>
-      <c r="E44" s="116"/>
+      <c r="E44" s="115"/>
       <c r="F44" s="44" t="s">
         <v>21</v>
       </c>
@@ -2692,10 +2700,10 @@
       <c r="E52" s="33"/>
       <c r="F52" s="33"/>
       <c r="G52" s="33"/>
-      <c r="H52" s="109" t="s">
+      <c r="H52" s="108" t="s">
         <v>14</v>
       </c>
-      <c r="I52" s="109"/>
+      <c r="I52" s="108"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" s="68" t="s">
@@ -2711,10 +2719,10 @@
       <c r="E53" s="71"/>
       <c r="F53" s="39"/>
       <c r="G53" s="39"/>
-      <c r="H53" s="110" t="s">
+      <c r="H53" s="109" t="s">
         <v>13</v>
       </c>
-      <c r="I53" s="110"/>
+      <c r="I53" s="109"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="O54" s="58"/>

</xml_diff>

<commit_message>
verifica scrittura mA su verbale
</commit_message>
<xml_diff>
--- a/other/T0XXX.xlsx
+++ b/other/T0XXX.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Progetti\Interfaccia Mu.De. Manager\Mu.De.Manager\sv_Mu.De.Manager\Mu.De._Manager\other\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\progetti\Interfaccia Mu.De. Manager\Mu.De.Manager\sv_Mu.De.Manager\Mu.De._Manager\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49509EFC-F874-4516-9BB4-18CD83EFC4C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C451D241-3D7B-4B78-ADDB-9CEE69C4AB42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="480" windowWidth="17115" windowHeight="8790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="48">
   <si>
     <t>F.P.</t>
   </si>
@@ -158,6 +158,12 @@
   </si>
   <si>
     <t>gg.mm.aaaa</t>
+  </si>
+  <si>
+    <t>146.40</t>
+  </si>
+  <si>
+    <t>144.90</t>
   </si>
 </sst>
 </file>
@@ -764,6 +770,15 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -832,15 +847,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1695,26 +1701,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="99"/>
-      <c r="B1" s="99"/>
-      <c r="C1" s="100" t="s">
+      <c r="A1" s="102"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="103" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="103"/>
+      <c r="G1" s="103"/>
     </row>
     <row r="2" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="27"/>
       <c r="B2" s="27"/>
       <c r="C2" s="28"/>
       <c r="D2" s="28"/>
-      <c r="E2" s="104" t="s">
+      <c r="E2" s="107" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="104"/>
-      <c r="G2" s="104"/>
+      <c r="F2" s="107"/>
+      <c r="G2" s="107"/>
     </row>
     <row r="3" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="70" t="s">
@@ -1724,24 +1730,24 @@
         <v>12</v>
       </c>
       <c r="C3" s="30"/>
-      <c r="D3" s="97" t="s">
+      <c r="D3" s="100" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
       <c r="G3" s="49" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="31"/>
-      <c r="B4" s="105" t="s">
+      <c r="B4" s="108" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="105"/>
-      <c r="D4" s="105"/>
-      <c r="E4" s="105"/>
-      <c r="F4" s="105"/>
+      <c r="C4" s="108"/>
+      <c r="D4" s="108"/>
+      <c r="E4" s="108"/>
+      <c r="F4" s="108"/>
       <c r="G4" s="50"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -1757,15 +1763,15 @@
       <c r="G5" s="38"/>
     </row>
     <row r="6" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="101" t="s">
+      <c r="A6" s="104" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="102"/>
-      <c r="C6" s="102"/>
-      <c r="D6" s="102"/>
-      <c r="E6" s="102"/>
-      <c r="F6" s="102"/>
-      <c r="G6" s="103"/>
+      <c r="B6" s="105"/>
+      <c r="C6" s="105"/>
+      <c r="D6" s="105"/>
+      <c r="E6" s="105"/>
+      <c r="F6" s="105"/>
+      <c r="G6" s="106"/>
     </row>
     <row r="7" spans="1:10" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
@@ -1791,9 +1797,9 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="98"/>
-      <c r="B9" s="98"/>
-      <c r="C9" s="98"/>
+      <c r="A9" s="101"/>
+      <c r="B9" s="101"/>
+      <c r="C9" s="101"/>
       <c r="D9" s="10"/>
       <c r="E9" s="51"/>
       <c r="F9" s="6"/>
@@ -1815,9 +1821,9 @@
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="98"/>
-      <c r="B11" s="98"/>
-      <c r="C11" s="98"/>
+      <c r="A11" s="101"/>
+      <c r="B11" s="101"/>
+      <c r="C11" s="101"/>
       <c r="D11" s="10"/>
       <c r="E11" s="51"/>
       <c r="F11" s="6"/>
@@ -1839,9 +1845,9 @@
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="98"/>
-      <c r="B13" s="98"/>
-      <c r="C13" s="98"/>
+      <c r="A13" s="101"/>
+      <c r="B13" s="101"/>
+      <c r="C13" s="101"/>
       <c r="D13" s="10"/>
       <c r="E13" s="51"/>
       <c r="F13" s="6"/>
@@ -1849,10 +1855,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="25"/>
-      <c r="B14" s="96" t="s">
+      <c r="B14" s="99" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="96"/>
+      <c r="C14" s="99"/>
       <c r="D14" s="12" t="s">
         <v>6</v>
       </c>
@@ -1877,10 +1883,10 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="25"/>
-      <c r="B16" s="96" t="s">
+      <c r="B16" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="96"/>
+      <c r="C16" s="99"/>
       <c r="D16" s="12" t="s">
         <v>6</v>
       </c>
@@ -1895,9 +1901,9 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="98"/>
-      <c r="B17" s="98"/>
-      <c r="C17" s="98"/>
+      <c r="A17" s="101"/>
+      <c r="B17" s="101"/>
+      <c r="C17" s="101"/>
       <c r="D17" s="10"/>
       <c r="E17" s="51"/>
       <c r="F17" s="6"/>
@@ -1907,10 +1913,10 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="25"/>
-      <c r="B18" s="96" t="s">
+      <c r="B18" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="96"/>
+      <c r="C18" s="99"/>
       <c r="D18" s="21" t="s">
         <v>10</v>
       </c>
@@ -1938,15 +1944,15 @@
       <c r="L19" s="57"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="107"/>
-      <c r="B20" s="107"/>
-      <c r="C20" s="107"/>
+      <c r="A20" s="110"/>
+      <c r="B20" s="110"/>
+      <c r="C20" s="110"/>
       <c r="D20" s="7"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="106"/>
-      <c r="I20" s="106"/>
+      <c r="H20" s="109"/>
+      <c r="I20" s="109"/>
       <c r="J20" s="57"/>
       <c r="L20" s="57"/>
     </row>
@@ -1963,10 +1969,10 @@
       <c r="D21" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="117" t="s">
+      <c r="E21" s="120" t="s">
         <v>38</v>
       </c>
-      <c r="F21" s="118"/>
+      <c r="F21" s="121"/>
       <c r="G21" s="88" t="s">
         <v>39</v>
       </c>
@@ -2137,7 +2143,9 @@
       <c r="I26" s="86">
         <v>3900</v>
       </c>
-      <c r="J26" s="95"/>
+      <c r="J26" s="95" t="s">
+        <v>46</v>
+      </c>
       <c r="L26" s="57"/>
       <c r="M26"/>
     </row>
@@ -2233,7 +2241,7 @@
       <c r="I29" s="87">
         <v>4100</v>
       </c>
-      <c r="J29" s="119"/>
+      <c r="J29" s="96"/>
       <c r="L29" s="57"/>
       <c r="M29"/>
     </row>
@@ -2247,7 +2255,7 @@
       <c r="G30" s="80"/>
       <c r="H30" s="82"/>
       <c r="I30" s="93"/>
-      <c r="J30" s="120" t="s">
+      <c r="J30" s="97" t="s">
         <v>26</v>
       </c>
       <c r="L30" s="57"/>
@@ -2273,7 +2281,7 @@
         <v>1.3</v>
       </c>
       <c r="G31" s="83">
-        <v>3510</v>
+        <v>3435</v>
       </c>
       <c r="H31" s="84">
         <v>3200</v>
@@ -2281,7 +2289,9 @@
       <c r="I31" s="85">
         <v>3800</v>
       </c>
-      <c r="J31" s="94"/>
+      <c r="J31" s="94" t="s">
+        <v>47</v>
+      </c>
       <c r="L31" s="57"/>
       <c r="M31"/>
     </row>
@@ -2345,7 +2355,7 @@
       <c r="I33" s="86">
         <v>3900</v>
       </c>
-      <c r="J33" s="121"/>
+      <c r="J33" s="98"/>
       <c r="L33" s="57"/>
       <c r="M33"/>
     </row>
@@ -2377,7 +2387,7 @@
       <c r="I34" s="86">
         <v>3900</v>
       </c>
-      <c r="J34" s="121"/>
+      <c r="J34" s="98"/>
       <c r="L34" s="57"/>
       <c r="M34"/>
     </row>
@@ -2409,7 +2419,7 @@
       <c r="I35" s="86">
         <v>4000</v>
       </c>
-      <c r="J35" s="121"/>
+      <c r="J35" s="98"/>
       <c r="L35" s="57"/>
       <c r="M35"/>
     </row>
@@ -2441,7 +2451,7 @@
       <c r="I36" s="86">
         <v>4000</v>
       </c>
-      <c r="J36" s="121"/>
+      <c r="J36" s="98"/>
       <c r="L36" s="57"/>
       <c r="M36"/>
     </row>
@@ -2473,7 +2483,7 @@
       <c r="I37" s="86">
         <v>4200</v>
       </c>
-      <c r="J37" s="121"/>
+      <c r="J37" s="98"/>
       <c r="L37" s="57"/>
       <c r="M37"/>
     </row>
@@ -2505,7 +2515,7 @@
       <c r="I38" s="86">
         <v>4300</v>
       </c>
-      <c r="J38" s="121"/>
+      <c r="J38" s="98"/>
       <c r="L38" s="57"/>
       <c r="M38"/>
     </row>
@@ -2569,7 +2579,7 @@
       <c r="I40" s="87">
         <v>4300</v>
       </c>
-      <c r="J40" s="119"/>
+      <c r="J40" s="96"/>
       <c r="L40" s="57"/>
       <c r="M40"/>
     </row>
@@ -2586,27 +2596,27 @@
     </row>
     <row r="42" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="43"/>
-      <c r="B42" s="116" t="s">
+      <c r="B42" s="119" t="s">
         <v>16</v>
       </c>
-      <c r="C42" s="116"/>
-      <c r="D42" s="116"/>
-      <c r="E42" s="116"/>
-      <c r="F42" s="116"/>
-      <c r="G42" s="116"/>
+      <c r="C42" s="119"/>
+      <c r="D42" s="119"/>
+      <c r="E42" s="119"/>
+      <c r="F42" s="119"/>
+      <c r="G42" s="119"/>
       <c r="H42" s="40"/>
       <c r="I42" s="41"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A43" s="111" t="s">
+      <c r="A43" s="114" t="s">
         <v>34</v>
       </c>
-      <c r="B43" s="112"/>
-      <c r="C43" s="112"/>
-      <c r="D43" s="110" t="s">
+      <c r="B43" s="115"/>
+      <c r="C43" s="115"/>
+      <c r="D43" s="113" t="s">
         <v>17</v>
       </c>
-      <c r="E43" s="110"/>
+      <c r="E43" s="113"/>
       <c r="F43" s="7" t="s">
         <v>19</v>
       </c>
@@ -2616,15 +2626,15 @@
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A44" s="113" t="s">
+      <c r="A44" s="116" t="s">
         <v>18</v>
       </c>
-      <c r="B44" s="114"/>
-      <c r="C44" s="114"/>
-      <c r="D44" s="115" t="s">
+      <c r="B44" s="117"/>
+      <c r="C44" s="117"/>
+      <c r="D44" s="118" t="s">
         <v>20</v>
       </c>
-      <c r="E44" s="115"/>
+      <c r="E44" s="118"/>
       <c r="F44" s="44" t="s">
         <v>21</v>
       </c>
@@ -2700,10 +2710,10 @@
       <c r="E52" s="33"/>
       <c r="F52" s="33"/>
       <c r="G52" s="33"/>
-      <c r="H52" s="108" t="s">
+      <c r="H52" s="111" t="s">
         <v>14</v>
       </c>
-      <c r="I52" s="108"/>
+      <c r="I52" s="111"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" s="68" t="s">
@@ -2719,10 +2729,10 @@
       <c r="E53" s="71"/>
       <c r="F53" s="39"/>
       <c r="G53" s="39"/>
-      <c r="H53" s="109" t="s">
+      <c r="H53" s="112" t="s">
         <v>13</v>
       </c>
-      <c r="I53" s="109"/>
+      <c r="I53" s="112"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="O54" s="58"/>

</xml_diff>